<commit_message>
ultima do ano... ou nao
</commit_message>
<xml_diff>
--- a/Cronogramas/Cronograma_Reuni�o_25_10_2011.xlsx
+++ b/Cronogramas/Cronograma_Reuni�o_25_10_2011.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="19035" windowHeight="8445"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="15270" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>Metas – Reunião 25/10 – 09:00 às 10:00</t>
   </si>
@@ -108,13 +108,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -122,6 +119,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -132,9 +133,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -172,7 +173,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -242,7 +243,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -416,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -427,127 +428,141 @@
     <col min="1" max="1" width="44.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="45">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="3" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="30">
-      <c r="A7" s="3" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>